<commit_message>
Partial completion of time based plots.
</commit_message>
<xml_diff>
--- a/src/Python/ddosi/units/Units.xlsx
+++ b/src/Python/ddosi/units/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Research Post Processor\src\Python\ddosi\units\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C26ED73-0D73-427F-8DA7-597CD8D85F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED325A1-0EA7-4D5F-9510-7F12EACA0ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="241">
   <si>
     <t>Data type</t>
   </si>
@@ -125,9 +125,6 @@
     <t>mm²</t>
   </si>
   <si>
-    <t>mm/rev</t>
-  </si>
-  <si>
     <t>deg/mm</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>m/rev/N</t>
   </si>
   <si>
-    <t>m/rad</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -353,9 +347,6 @@
     <t>usg/ft</t>
   </si>
   <si>
-    <t>inch/rev</t>
-  </si>
-  <si>
     <t>deg/inch</t>
   </si>
   <si>
@@ -665,9 +656,6 @@
     <t>torque</t>
   </si>
   <si>
-    <t>torque/weight</t>
-  </si>
-  <si>
     <t>torsional damping</t>
   </si>
   <si>
@@ -746,9 +734,6 @@
     <t>W/(m*°C)</t>
   </si>
   <si>
-    <t>kgf*m/tf</t>
-  </si>
-  <si>
     <t>kgf*m/rpm</t>
   </si>
   <si>
@@ -767,13 +752,13 @@
     <t>BTU/(hr*ft*°F)</t>
   </si>
   <si>
-    <t>lbf*ft/klbf</t>
-  </si>
-  <si>
     <t>lbf*ft/rpm</t>
   </si>
   <si>
     <t>lbf*inch/ft</t>
+  </si>
+  <si>
+    <t>inch/revolution</t>
   </si>
 </sst>
 </file>
@@ -1415,6 +1400,29 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1442,167 +1450,6 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1696,6 +1543,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -1708,6 +1571,128 @@
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1796,56 +1781,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{91A77D04-7425-4B71-8F47-33EF5473D73D}" name="Table5" displayName="Table5" ref="A1:B90" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A1:B90" xr:uid="{91A77D04-7425-4B71-8F47-33EF5473D73D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B90">
-    <sortCondition ref="A1:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{91A77D04-7425-4B71-8F47-33EF5473D73D}" name="Table5" displayName="Table5" ref="A1:B89" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:B89" xr:uid="{91A77D04-7425-4B71-8F47-33EF5473D73D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
+    <sortCondition ref="A1:A89"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{041CD49B-55BF-46D9-AB1F-5C1610C89002}" name="Data type" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A55AA01D-5B74-4CE6-8F94-A29E93E0C289}" name="Unit" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{041CD49B-55BF-46D9-AB1F-5C1610C89002}" name="Data type" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A55AA01D-5B74-4CE6-8F94-A29E93E0C289}" name="Unit" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0F89EC03-9CED-46AD-8B80-5F690F3A3A46}" name="Table4" displayName="Table4" ref="A1:B90" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:B90" xr:uid="{0F89EC03-9CED-46AD-8B80-5F690F3A3A46}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B90">
-    <sortCondition ref="A1:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0F89EC03-9CED-46AD-8B80-5F690F3A3A46}" name="Table4" displayName="Table4" ref="A1:B89" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:B89" xr:uid="{0F89EC03-9CED-46AD-8B80-5F690F3A3A46}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
+    <sortCondition ref="A1:A89"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{039F433C-E552-4734-A65B-D7B152F1ADF7}" name="Data type" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{066B27F1-795E-446D-973D-F2F834BCE227}" name="Unit" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{039F433C-E552-4734-A65B-D7B152F1ADF7}" name="Data type" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{066B27F1-795E-446D-973D-F2F834BCE227}" name="Unit" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E630DBA4-2EF5-477A-8382-432FFCA00DFD}" name="Table2" displayName="Table2" ref="A1:B90" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:B90" xr:uid="{E630DBA4-2EF5-477A-8382-432FFCA00DFD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B90">
-    <sortCondition ref="A1:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E630DBA4-2EF5-477A-8382-432FFCA00DFD}" name="Table2" displayName="Table2" ref="A1:B89" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:B89" xr:uid="{E630DBA4-2EF5-477A-8382-432FFCA00DFD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
+    <sortCondition ref="A1:A89"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E2181ECB-5E33-401B-BC99-62B3A887CEF0}" name="Data type" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{0DD98A30-62AB-40BE-902B-9CE6ABF0FA24}" name="Unit" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{E2181ECB-5E33-401B-BC99-62B3A887CEF0}" name="Data type" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0DD98A30-62AB-40BE-902B-9CE6ABF0FA24}" name="Unit" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{24938835-2BF0-425C-BACE-FDDC50D91FEF}" name="Table3" displayName="Table3" ref="A1:B90" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:B90" xr:uid="{24938835-2BF0-425C-BACE-FDDC50D91FEF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B90">
-    <sortCondition ref="A1:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{24938835-2BF0-425C-BACE-FDDC50D91FEF}" name="Table3" displayName="Table3" ref="A1:B89" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B89" xr:uid="{24938835-2BF0-425C-BACE-FDDC50D91FEF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
+    <sortCondition ref="A1:A89"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{96BC98BA-7F61-49D8-ACE3-3FB8FA21D406}" name="Data type" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D93D8364-01D8-4A4B-B9BD-4CEED4784731}" name="Unit" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{96BC98BA-7F61-49D8-ACE3-3FB8FA21D406}" name="Data type" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D93D8364-01D8-4A4B-B9BD-4CEED4784731}" name="Unit" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2148,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1BF487-369A-4722-BB28-2CCD37AAB7E0}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,47 +2155,47 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -2218,7 +2203,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -2226,73 +2211,73 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
@@ -2300,7 +2285,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
@@ -2308,15 +2293,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
@@ -2324,23 +2309,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
@@ -2348,55 +2333,55 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>3</v>
@@ -2404,23 +2389,23 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>3</v>
@@ -2428,63 +2413,63 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>24</v>
@@ -2492,23 +2477,23 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
@@ -2516,7 +2501,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>27</v>
@@ -2524,7 +2509,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>17</v>
@@ -2532,31 +2517,31 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>17</v>
@@ -2564,7 +2549,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>2</v>
@@ -2572,7 +2557,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>3</v>
@@ -2580,15 +2565,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>21</v>
@@ -2596,15 +2581,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>2</v>
@@ -2612,7 +2597,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>19</v>
@@ -2620,71 +2605,71 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>71</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>2</v>
@@ -2692,7 +2677,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>26</v>
@@ -2700,71 +2685,71 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>3</v>
@@ -2772,7 +2757,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>26</v>
@@ -2780,98 +2765,90 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>226</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>232</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2884,10 +2861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1677F27-80CD-4A2F-AA13-AC314276127A}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,7 +2883,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -2914,15 +2891,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -2930,15 +2907,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -2946,7 +2923,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -2954,7 +2931,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -2962,51 +2939,51 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -3014,13 +2991,13 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
@@ -3028,7 +3005,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
@@ -3036,7 +3013,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
@@ -3044,15 +3021,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -3060,7 +3037,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -3068,15 +3045,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
@@ -3084,7 +3061,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
@@ -3092,7 +3069,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -3100,23 +3077,23 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>14</v>
@@ -3124,15 +3101,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>11</v>
@@ -3140,7 +3117,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>13</v>
@@ -3148,7 +3125,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>22</v>
@@ -3156,7 +3133,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>3</v>
@@ -3164,39 +3141,39 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>25</v>
@@ -3204,23 +3181,23 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>24</v>
@@ -3228,23 +3205,23 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
@@ -3252,15 +3229,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>17</v>
@@ -3268,31 +3245,31 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>16</v>
@@ -3300,7 +3277,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>2</v>
@@ -3308,15 +3285,15 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>8</v>
@@ -3324,7 +3301,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>21</v>
@@ -3332,7 +3309,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>6</v>
@@ -3340,7 +3317,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>2</v>
@@ -3348,7 +3325,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>19</v>
@@ -3356,7 +3333,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>22</v>
@@ -3364,15 +3341,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>13</v>
@@ -3380,7 +3357,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
@@ -3388,39 +3365,39 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>2</v>
@@ -3428,7 +3405,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>26</v>
@@ -3436,15 +3413,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>22</v>
@@ -3452,7 +3429,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>20</v>
@@ -3460,47 +3437,47 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>15</v>
@@ -3508,7 +3485,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>26</v>
@@ -3516,98 +3493,90 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>237</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>35</v>
+      <c r="A89" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3620,10 +3589,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B5E0A5-F1C5-433D-956C-148C241EA4A5}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,23 +3611,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -3666,15 +3635,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -3682,7 +3651,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -3690,7 +3659,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -3698,51 +3667,51 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -3750,29 +3719,29 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
@@ -3780,15 +3749,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
@@ -3796,31 +3765,31 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>12</v>
@@ -3828,47 +3797,47 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>11</v>
@@ -3876,7 +3845,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
@@ -3884,159 +3853,159 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>2</v>
@@ -4044,23 +4013,23 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>21</v>
@@ -4068,15 +4037,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>2</v>
@@ -4084,7 +4053,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>19</v>
@@ -4092,23 +4061,23 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>13</v>
@@ -4116,7 +4085,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>9</v>
@@ -4124,39 +4093,39 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>2</v>
@@ -4164,7 +4133,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>26</v>
@@ -4172,71 +4141,71 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>11</v>
@@ -4244,7 +4213,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>26</v>
@@ -4252,98 +4221,90 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>244</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>218</v>
+      <c r="A89" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4356,10 +4317,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2699DA-8C2F-4310-9FA4-9E62DDBB2114}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4378,7 +4339,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -4386,15 +4347,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -4402,15 +4363,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -4418,7 +4379,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -4426,7 +4387,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -4434,51 +4395,51 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -4486,21 +4447,21 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
@@ -4508,7 +4469,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
@@ -4516,15 +4477,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
@@ -4532,7 +4493,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -4540,15 +4501,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
@@ -4556,7 +4517,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
@@ -4564,47 +4525,47 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>15</v>
@@ -4612,7 +4573,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>13</v>
@@ -4620,15 +4581,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>3</v>
@@ -4636,39 +4597,39 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>25</v>
@@ -4676,23 +4637,23 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>24</v>
@@ -4700,23 +4661,23 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
@@ -4724,15 +4685,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>17</v>
@@ -4740,39 +4701,39 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>2</v>
@@ -4780,15 +4741,15 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>8</v>
@@ -4796,7 +4757,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>21</v>
@@ -4804,15 +4765,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>2</v>
@@ -4820,7 +4781,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>19</v>
@@ -4828,7 +4789,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>22</v>
@@ -4836,15 +4797,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>13</v>
@@ -4852,7 +4813,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
@@ -4860,39 +4821,39 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>29</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>2</v>
@@ -4900,7 +4861,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>26</v>
@@ -4908,15 +4869,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>22</v>
@@ -4924,7 +4885,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>20</v>
@@ -4932,47 +4893,47 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>15</v>
@@ -4980,7 +4941,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>26</v>
@@ -4988,97 +4949,89 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>222</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="5" t="s">
+      <c r="A89" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Configure Pint to use custom definitions.
</commit_message>
<xml_diff>
--- a/src/Python/ddosi/units/Units.xlsx
+++ b/src/Python/ddosi/units/Units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Research Post Processor\src\Python\ddosi\units\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED325A1-0EA7-4D5F-9510-7F12EACA0ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99FF5DF-6795-4C63-9CB9-893C7F7352C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="242">
   <si>
     <t>Data type</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>inch/revolution</t>
+  </si>
+  <si>
+    <t>gravity</t>
   </si>
 </sst>
 </file>
@@ -2135,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1BF487-369A-4722-BB28-2CCD37AAB7E0}">
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD80"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1677F27-80CD-4A2F-AA13-AC314276127A}">
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD80"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2897,7 @@
         <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>